<commit_message>
Updated README and excel lg
</commit_message>
<xml_diff>
--- a/blind_75.xlsx
+++ b/blind_75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmeadejr./Desktop/Programming/Study/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D425875-DDD9-0443-844A-8B3585CD015C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0E000A-A80D-574F-ADD1-C2AD8F0A42F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{56A7C0B3-866D-4D41-ACE2-0A67D57CC61F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Category</t>
   </si>
@@ -62,13 +62,7 @@
     <t>BF Solution</t>
   </si>
   <si>
-    <t>BF Notes</t>
-  </si>
-  <si>
     <t>MO Solution</t>
-  </si>
-  <si>
-    <t>MO Notes</t>
   </si>
   <si>
     <t>BF Time Complexity</t>
@@ -113,6 +107,15 @@
   </si>
   <si>
     <t>If each element in your input requires a loop over all other elements, the time complexity is likely O(n^2).</t>
+  </si>
+  <si>
+    <t>BF Approach</t>
+  </si>
+  <si>
+    <t>MO Approach</t>
+  </si>
+  <si>
+    <t>https://github.com/davidmeadejr/leetcode/blob/main/blind_75/array/brute_force/two_sum.py</t>
   </si>
 </sst>
 </file>
@@ -178,12 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -517,26 +519,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E14A61B-163D-E54D-91D0-AF7B0EADC8D8}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,58 +556,60 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
-      <c r="G7" s="1"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Corrected two sum brute force solution
</commit_message>
<xml_diff>
--- a/blind_75.xlsx
+++ b/blind_75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmeadejr./Desktop/Programming/Study/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0E000A-A80D-574F-ADD1-C2AD8F0A42F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97606627-2C21-7743-BDC1-3D9FC9DB59F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{56A7C0B3-866D-4D41-ACE2-0A67D57CC61F}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>